<commit_message>
divide preparation into three stages
</commit_message>
<xml_diff>
--- a/hh_video_data.xlsx
+++ b/hh_video_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,51 +37,52 @@
     <t xml:space="preserve">frame_length</t>
   </si>
   <si>
-    <t xml:space="preserve">num_of_frames</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20180806_1</t>
+    <t xml:space="preserve">1_20180806</t>
   </si>
   <si>
     <t xml:space="preserve">710, 865, 910, 1040, 1100, 1130, 1210, 1370, 1400, 1460, 1540, 1600</t>
   </si>
   <si>
-    <t xml:space="preserve">20180920_2</t>
+    <t xml:space="preserve">2_20180920</t>
   </si>
   <si>
     <t xml:space="preserve">215, 325</t>
   </si>
   <si>
-    <t xml:space="preserve">20180920_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20180920_4</t>
+    <t xml:space="preserve">3_20180920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4_20180920</t>
   </si>
   <si>
     <t xml:space="preserve">160, 175, 190, 300, 415, 430, 445</t>
   </si>
   <si>
-    <t xml:space="preserve">20180920_5</t>
+    <t xml:space="preserve">5_20180920</t>
   </si>
   <si>
     <t xml:space="preserve">215, 275, 465, 480, 600</t>
   </si>
   <si>
-    <t xml:space="preserve">20180920_6</t>
+    <t xml:space="preserve">6_20180920</t>
   </si>
   <si>
     <t xml:space="preserve">1190, 1490, 1795</t>
   </si>
   <si>
-    <t xml:space="preserve">20180920_7</t>
+    <t xml:space="preserve">7_20180920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200, 215, 270, 465, 480, 590, 605</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -148,8 +149,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,18 +183,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -201,11 +212,8 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -213,19 +221,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>20180806</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>30</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>1718</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -233,19 +238,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>20180920</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>20180920</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>373</v>
+      <c r="E3" s="2" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -253,16 +255,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>20180920</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>300</v>
+      <c r="E4" s="2" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,19 +269,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>20180920</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>20180920</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>572</v>
+      <c r="E5" s="2" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,19 +286,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>20180920</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>20180920</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>651</v>
+      <c r="E6" s="2" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -310,19 +303,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>20180920</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="n">
         <v>60</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>1663</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -330,10 +320,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>20180920</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>20180920</v>
+      <c r="E8" s="1" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>